<commit_message>
Added 'Foreigners' as a datafield
</commit_message>
<xml_diff>
--- a/Dataset/Dataset - January (Template).xlsx
+++ b/Dataset/Dataset - January (Template).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vvaseekaran/Desktop/Datathon-COVID/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B77D31-9D90-AF49-8637-6E4B26FD49A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3818A53E-A2B7-524D-83EB-6F4E1EC7C003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{91FEF145-7FEC-AC40-BFC3-122113799E9A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Colombo</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Galle</t>
+  </si>
+  <si>
+    <t>Foreigners</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BEC1DA-5774-074F-9F07-F4B2FCD8AAE4}">
-  <dimension ref="A1:AA33"/>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +513,7 @@
     <col min="25" max="25" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
@@ -555,7 +558,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -637,8 +640,11 @@
       <c r="AA2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -646,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -654,7 +660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -662,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -670,7 +676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -678,7 +684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -686,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -694,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -702,7 +708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -710,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -718,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -726,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -734,7 +740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -742,7 +748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>